<commit_message>
Au final création d'un fichier merge.xlsx avec le script python pour extraires les infod du pdf. Le fichier Feuille de travail récupere par macro le contenu de ce fichier. Voir pour lancer le script python par vba (fichier .bat) puis récup les valeurs A finir : Récuperer la listes des echantillons avec les pesées pour créer le fichier ICP
</commit_message>
<xml_diff>
--- a/merge.xlsx
+++ b/merge.xlsx
@@ -1,36 +1,182 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Partage\PycharmProjects\pdftoexcel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4A20E3-4CF1-42E6-B695-496A813508AE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Config" sheetId="2" r:id="rId1"/>
+    <sheet name="07-11-18" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Test</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Famille</t>
+  </si>
+  <si>
+    <t>Nuance</t>
+  </si>
+  <si>
+    <t>Identifiant échantillon</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>Réacteur</t>
+  </si>
+  <si>
+    <t>Fiole</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Délai</t>
+  </si>
+  <si>
+    <t>R. Acier I</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>R. Inco I</t>
+  </si>
+  <si>
+    <t>INOXYDABLES</t>
+  </si>
+  <si>
+    <t>ALLIES</t>
+  </si>
+  <si>
+    <t>DIVERS</t>
+  </si>
+  <si>
+    <t>316-201LN</t>
+  </si>
+  <si>
+    <t>UR31</t>
+  </si>
+  <si>
+    <t>X65</t>
+  </si>
+  <si>
+    <t>625</t>
+  </si>
+  <si>
+    <t>13FSU125</t>
+  </si>
+  <si>
+    <t>13FSU25</t>
+  </si>
+  <si>
+    <t>UR65</t>
+  </si>
+  <si>
+    <t>1439444-992</t>
+  </si>
+  <si>
+    <t>1439444-993</t>
+  </si>
+  <si>
+    <t>1439699-994</t>
+  </si>
+  <si>
+    <t>1439699-995</t>
+  </si>
+  <si>
+    <t>1440279-968</t>
+  </si>
+  <si>
+    <t>1440279-969</t>
+  </si>
+  <si>
+    <t>1440279-970</t>
+  </si>
+  <si>
+    <t>1440278-971</t>
+  </si>
+  <si>
+    <t>1440278-972</t>
+  </si>
+  <si>
+    <t>1440278-973</t>
+  </si>
+  <si>
+    <t>1190551-2947</t>
+  </si>
+  <si>
+    <t>B184364-1006</t>
+  </si>
+  <si>
+    <t>B184355-1007</t>
+  </si>
+  <si>
+    <t>A183309-1011</t>
+  </si>
+  <si>
+    <t>MD 316 DILUE  201LN</t>
+  </si>
+  <si>
+    <t>MD 316 DILUE 201LN</t>
+  </si>
+  <si>
+    <t>MO &gt;6%</t>
+  </si>
+  <si>
+    <t>BBT</t>
+  </si>
+  <si>
+    <t>32853</t>
+  </si>
+  <si>
+    <t>32854</t>
+  </si>
+  <si>
+    <t>32859</t>
+  </si>
+  <si>
+    <t>08/11/2018</t>
+  </si>
+  <si>
+    <t>15/11/2018</t>
+  </si>
+  <si>
+    <t>07/11/2018</t>
+  </si>
+  <si>
+    <t>06/09/2018</t>
+  </si>
+  <si>
+    <t>05/11/2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -54,26 +200,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -361,18 +517,424 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8112A925-F294-4B2E-BA35-E166874C2261}">
-  <dimension ref="B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Voir pour finir en ajoutant le contenue de test.py => execution de la macro excel par python
</commit_message>
<xml_diff>
--- a/merge.xlsx
+++ b/merge.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="07-11-18" sheetId="1" r:id="rId1"/>
+    <sheet name="07-11-18" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Type</t>
   </si>
@@ -46,147 +47,143 @@
     <t>R. Acier I</t>
   </si>
   <si>
+    <t>INOXYDABLES</t>
+  </si>
+  <si>
+    <t>316-201LN</t>
+  </si>
+  <si>
+    <t>1439444-992</t>
+  </si>
+  <si>
+    <t>MD 316 DILUE  201LN</t>
+  </si>
+  <si>
+    <t>08/11/2018</t>
+  </si>
+  <si>
+    <t>1439444-993</t>
+  </si>
+  <si>
+    <t>MD 316 DILUE 201LN</t>
+  </si>
+  <si>
+    <t>UR31</t>
+  </si>
+  <si>
+    <t>1439699-994</t>
+  </si>
+  <si>
+    <t>15/11/2018</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
     <t>Ca</t>
   </si>
   <si>
+    <t>1439699-995</t>
+  </si>
+  <si>
+    <t>MO &gt;6%</t>
+  </si>
+  <si>
+    <t>ALLIES</t>
+  </si>
+  <si>
+    <t>X65</t>
+  </si>
+  <si>
+    <t>1440279-968</t>
+  </si>
+  <si>
+    <t>BBT</t>
+  </si>
+  <si>
+    <t>07/11/2018</t>
+  </si>
+  <si>
+    <t>1440279-969</t>
+  </si>
+  <si>
+    <t>1440279-970</t>
+  </si>
+  <si>
+    <t>1440278-971</t>
+  </si>
+  <si>
+    <t>1440278-972</t>
+  </si>
+  <si>
+    <t>1440278-973</t>
+  </si>
+  <si>
     <t>R. Inco I</t>
   </si>
   <si>
-    <t>INOXYDABLES</t>
-  </si>
-  <si>
-    <t>ALLIES</t>
-  </si>
-  <si>
     <t>DIVERS</t>
   </si>
   <si>
-    <t>316-201LN</t>
-  </si>
-  <si>
-    <t>UR31</t>
-  </si>
-  <si>
-    <t>X65</t>
-  </si>
-  <si>
     <t>625</t>
   </si>
   <si>
+    <t>1190551-2947</t>
+  </si>
+  <si>
+    <t>06/09/2018</t>
+  </si>
+  <si>
     <t>13FSU125</t>
   </si>
   <si>
+    <t>B184364-1006</t>
+  </si>
+  <si>
+    <t>32853</t>
+  </si>
+  <si>
+    <t>05/11/2018</t>
+  </si>
+  <si>
     <t>13FSU25</t>
   </si>
   <si>
+    <t>B184355-1007</t>
+  </si>
+  <si>
+    <t>32854</t>
+  </si>
+  <si>
     <t>UR65</t>
   </si>
   <si>
-    <t>1439444-992</t>
-  </si>
-  <si>
-    <t>1439444-993</t>
-  </si>
-  <si>
-    <t>1439699-994</t>
-  </si>
-  <si>
-    <t>1439699-995</t>
-  </si>
-  <si>
-    <t>1440279-968</t>
-  </si>
-  <si>
-    <t>1440279-969</t>
-  </si>
-  <si>
-    <t>1440279-970</t>
-  </si>
-  <si>
-    <t>1440278-971</t>
-  </si>
-  <si>
-    <t>1440278-972</t>
-  </si>
-  <si>
-    <t>1440278-973</t>
-  </si>
-  <si>
-    <t>1190551-2947</t>
-  </si>
-  <si>
-    <t>B184364-1006</t>
-  </si>
-  <si>
-    <t>B184355-1007</t>
-  </si>
-  <si>
     <t>A183309-1011</t>
   </si>
   <si>
-    <t>MD 316 DILUE  201LN</t>
-  </si>
-  <si>
-    <t>MD 316 DILUE 201LN</t>
-  </si>
-  <si>
-    <t>MO &gt;6%</t>
-  </si>
-  <si>
-    <t>BBT</t>
-  </si>
-  <si>
-    <t>32853</t>
-  </si>
-  <si>
-    <t>32854</t>
-  </si>
-  <si>
     <t>32859</t>
-  </si>
-  <si>
-    <t>08/11/2018</t>
-  </si>
-  <si>
-    <t>15/11/2018</t>
-  </si>
-  <si>
-    <t>07/11/2018</t>
-  </si>
-  <si>
-    <t>06/09/2018</t>
-  </si>
-  <si>
-    <t>05/11/2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -201,35 +198,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -517,12 +505,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
@@ -558,19 +552,22 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s"/>
+      <c r="F2" t="s"/>
+      <c r="G2" t="s"/>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>37</v>
-      </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -578,19 +575,22 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s"/>
+      <c r="F3" t="s"/>
+      <c r="G3" t="s"/>
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>38</v>
-      </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -598,38 +598,54 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E4" t="s"/>
+      <c r="F4" t="s"/>
+      <c r="G4" t="s"/>
+      <c r="H4" t="s"/>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B5" t="s"/>
+      <c r="C5" t="s"/>
       <c r="D5" t="s">
-        <v>25</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E5" t="s"/>
+      <c r="F5" t="s"/>
+      <c r="G5" t="s"/>
+      <c r="H5" t="s"/>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B6" t="s"/>
+      <c r="C6" t="s"/>
       <c r="D6" t="s">
-        <v>25</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E6" t="s"/>
+      <c r="F6" t="s"/>
+      <c r="G6" t="s"/>
+      <c r="H6" t="s"/>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -637,41 +653,56 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E7" t="s"/>
+      <c r="F7" t="s"/>
+      <c r="G7" t="s"/>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B8" t="s"/>
+      <c r="C8" t="s"/>
       <c r="D8" t="s">
-        <v>26</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E8" t="s"/>
+      <c r="F8" t="s"/>
+      <c r="G8" t="s"/>
+      <c r="H8" t="s"/>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B9" t="s"/>
+      <c r="C9" t="s"/>
       <c r="D9" t="s">
-        <v>26</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E9" t="s"/>
+      <c r="F9" t="s"/>
+      <c r="G9" t="s"/>
+      <c r="H9" t="s"/>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -679,30 +710,39 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s"/>
+      <c r="F10" t="s"/>
+      <c r="G10" t="s"/>
+      <c r="H10" t="s">
         <v>27</v>
       </c>
-      <c r="H10" t="s">
-        <v>40</v>
-      </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B11" t="s"/>
+      <c r="C11" t="s"/>
       <c r="D11" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E11" t="s"/>
+      <c r="F11" t="s"/>
+      <c r="G11" t="s"/>
+      <c r="H11" t="s"/>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -710,30 +750,39 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E12" t="s"/>
+      <c r="F12" t="s"/>
+      <c r="G12" t="s"/>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B13" t="s"/>
+      <c r="C13" t="s"/>
       <c r="D13" t="s">
-        <v>28</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E13" t="s"/>
+      <c r="F13" t="s"/>
+      <c r="G13" t="s"/>
+      <c r="H13" t="s"/>
       <c r="I13" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -741,30 +790,39 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E14" t="s"/>
+      <c r="F14" t="s"/>
+      <c r="G14" t="s"/>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B15" t="s"/>
+      <c r="C15" t="s"/>
       <c r="D15" t="s">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E15" t="s"/>
+      <c r="F15" t="s"/>
+      <c r="G15" t="s"/>
+      <c r="H15" t="s"/>
       <c r="I15" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -772,30 +830,39 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E16" t="s"/>
+      <c r="F16" t="s"/>
+      <c r="G16" t="s"/>
       <c r="H16" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I16" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B17" t="s"/>
+      <c r="C17" t="s"/>
       <c r="D17" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E17" t="s"/>
+      <c r="F17" t="s"/>
+      <c r="G17" t="s"/>
+      <c r="H17" t="s"/>
       <c r="I17" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -803,30 +870,39 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E18" t="s"/>
+      <c r="F18" t="s"/>
+      <c r="G18" t="s"/>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I18" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B19" t="s"/>
+      <c r="C19" t="s"/>
       <c r="D19" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E19" t="s"/>
+      <c r="F19" t="s"/>
+      <c r="G19" t="s"/>
+      <c r="H19" t="s"/>
       <c r="I19" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -834,110 +910,132 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E20" t="s"/>
+      <c r="F20" t="s"/>
+      <c r="G20" t="s"/>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I20" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s"/>
+      <c r="C21" t="s"/>
       <c r="D21" t="s">
-        <v>32</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E21" t="s"/>
+      <c r="F21" t="s"/>
+      <c r="G21" t="s"/>
+      <c r="H21" t="s"/>
       <c r="I21" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E22" t="s"/>
+      <c r="F22" t="s"/>
+      <c r="G22" t="s"/>
+      <c r="H22" t="s"/>
       <c r="I22" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E23" t="s"/>
+      <c r="F23" t="s"/>
+      <c r="G23" t="s"/>
       <c r="H23" t="s">
         <v>41</v>
       </c>
       <c r="I23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E24" t="s"/>
+      <c r="F24" t="s"/>
+      <c r="G24" t="s"/>
       <c r="H24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" t="s">
         <v>42</v>
-      </c>
-      <c r="I24" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E25" t="s"/>
+      <c r="F25" t="s"/>
+      <c r="G25" t="s"/>
       <c r="H25" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I25" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>